<commit_message>
Fixed: 7 and 14.1
</commit_message>
<xml_diff>
--- a/_document/Bug Collections - kha.xlsx
+++ b/_document/Bug Collections - kha.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
   <si>
     <t>1. Đưa group vào enable recommendation</t>
   </si>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BQ96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1228,6 +1228,9 @@
       </c>
       <c r="C9" s="12" t="s">
         <v>39</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:69">
@@ -2641,6 +2644,9 @@
       <c r="B41" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C41" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="42" spans="1:69">
       <c r="A42" s="14"/>
@@ -2718,7 +2724,7 @@
         <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D43" t="s">
         <v>33</v>
@@ -3650,7 +3656,12 @@
       <c r="B56" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E56" s="12"/>
+      <c r="C56" t="s">
+        <v>39</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>

</xml_diff>

<commit_message>
Sắp xếp thứ tự enable các plugin (recommended by SNORG). Chỉnh kích thước hình ảnh trong block fiends
</commit_message>
<xml_diff>
--- a/_document/Bug Collections - kha.xlsx
+++ b/_document/Bug Collections - kha.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
   <si>
     <t>1. Đưa group vào enable recommendation</t>
   </si>
@@ -512,15 +512,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2228850</xdr:colOff>
+      <xdr:colOff>2409825</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -538,7 +538,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="609600" y="3238500"/>
+          <a:off x="790575" y="3267075"/>
           <a:ext cx="2228850" cy="2057400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -839,13 +839,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BQ96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="64.85546875" customWidth="1"/>
+    <col min="2" max="2" width="76.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" customWidth="1"/>
@@ -1626,7 +1626,9 @@
       <c r="C16" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="12"/>
+      <c r="E16" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
@@ -3735,9 +3737,11 @@
         <v>20</v>
       </c>
       <c r="C57" t="s">
-        <v>34</v>
-      </c>
-      <c r="E57" s="12"/>
+        <v>39</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>

</xml_diff>

<commit_message>
Fix advancesearch: 12. Fix layout cho profile.
</commit_message>
<xml_diff>
--- a/_document/Bug Collections - kha.xlsx
+++ b/_document/Bug Collections - kha.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
   <si>
     <t>1. Đưa group vào enable recommendation</t>
   </si>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BQ96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2606,6 +2606,9 @@
       <c r="C30" t="s">
         <v>39</v>
       </c>
+      <c r="E30" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="31" spans="1:69">
       <c r="B31" s="1"/>

</xml_diff>